<commit_message>
drug usage as virtual column
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2017-2018.xlsx
+++ b/metadata/STR-NHANES-2017-2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F52DB39-7741-814C-BB7E-04F2E1FC7430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4996B323-E9E5-4943-8ED6-BA8648C224BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -114,22 +114,19 @@
     <t>topic</t>
   </si>
   <si>
+    <t>nhanes-kb:DPL-DSQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-DMQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>example@example.com</t>
+  </si>
+  <si>
+    <t>NHANES-2017-2018-RXQ_RX_J-T</t>
+  </si>
+  <si>
     <t>NHANES-2017-2018-RXQ_RX_J-P</t>
-  </si>
-  <si>
-    <t>NHANES-2017-2018-RXQ_RX_J-T</t>
-  </si>
-  <si>
-    <t>NHANES-2017-2018-RXQ_RX_J-E</t>
-  </si>
-  <si>
-    <t>nhanes-kb:DPL-DSQ_J-QUESTIONNAIRE</t>
-  </si>
-  <si>
-    <t>nhanes-kb:DPL-DMQ_J-QUESTIONNAIRE</t>
-  </si>
-  <si>
-    <t>example@example.com</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1543,74 +1540,57 @@
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E3:E5" r:id="rId2" display="example@example.com" xr:uid="{B553045A-7EE8-EC40-84DB-20EDEC23CC3F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{CA9EDFFF-9119-1F49-9CE7-5645C8131703}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{6D46E41A-4038-984A-9D5B-871B0E33439C}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
using single DEMO SDD
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2017-2018.xlsx
+++ b/metadata/STR-NHANES-2017-2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4996B323-E9E5-4943-8ED6-BA8648C224BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C70522-BDFA-8544-AD87-D5D421CA7FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>NHANES-2017-2018-RXQ_RX_J-P</t>
+  </si>
+  <si>
+    <t>NHANES-DEMO</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1501,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1537,7 +1540,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
lab results dara acquisitions
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2017-2018.xlsx
+++ b/metadata/STR-NHANES-2017-2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F117B787-03B9-6D4F-B070-897EEE0DC955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F859D-E29D-2245-ABB2-25B7BF297741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -139,13 +139,31 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-HIQ_J-QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>NHANES-2017-2018-TCHOL_J</t>
+  </si>
+  <si>
+    <t>NHANES-TCHOL</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
+  </si>
+  <si>
+    <t>NHANES-2017-2018-GLU_J</t>
+  </si>
+  <si>
+    <t>NHANES-GLU</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-C-ANALYZER-C311</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -167,6 +185,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -213,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -227,6 +251,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1507,17 +1532,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="65.1640625" style="5" customWidth="1"/>
@@ -1616,12 +1641,50 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{CA9EDFFF-9119-1F49-9CE7-5645C8131703}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{6D46E41A-4038-984A-9D5B-871B0E33439C}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B047EE7D-3A98-3546-BCE4-13D107937170}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{809F3561-BA15-7B47-8F3B-21921DB80D79}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{873AD8E1-2810-5B49-AAC7-F443E7C4DB3E}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
update STR with unified lab results SDD
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2017-2018.xlsx
+++ b/metadata/STR-NHANES-2017-2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72ACC6A-8357-9945-A9DE-2EDCA774EE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2A03D-3FD0-C94D-9CAE-F82D25A37C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -144,18 +144,12 @@
     <t>NHANES-2017-2018-TCHOL_J</t>
   </si>
   <si>
-    <t>NHANES-TCHOL</t>
-  </si>
-  <si>
     <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-6000-ANALYZER</t>
   </si>
   <si>
     <t>NHANES-2017-2018-GLU_J</t>
   </si>
   <si>
-    <t>NHANES-GLU</t>
-  </si>
-  <si>
     <t>nhanes-kb:DPL-ROCHE-HITACHI-COBAS-C-ANALYZER-C311</t>
   </si>
   <si>
@@ -171,10 +165,10 @@
     <t>NHANES-2017-2018-GHB_J</t>
   </si>
   <si>
-    <t>NHANES-GHB</t>
-  </si>
-  <si>
     <t>nhanes-kb:DPL-TOSOH-G8-GLYCOHEMOGLOBIN-ANALYZER</t>
+  </si>
+  <si>
+    <t>NHANES-LAB-RESULTS</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1547,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1589,13 +1583,13 @@
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="8" t="s">
@@ -1682,10 +1676,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="8" t="s">
@@ -1697,13 +1691,13 @@
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="8" t="s">
@@ -1715,13 +1709,13 @@
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>45</v>
-      </c>
       <c r="C9" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="8" t="s">

</xml_diff>

<commit_message>
updated DA to the unified SDD
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2017-2018.xlsx
+++ b/metadata/STR-NHANES-2017-2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2A03D-3FD0-C94D-9CAE-F82D25A37C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99BD410-F942-BB46-B229-0D1F32018A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>NHANES-LAB-RESULTS</t>
+  </si>
+  <si>
+    <t>NHANES-RXQ_RX-T</t>
+  </si>
+  <si>
+    <t>NHANES-RXQ_RX-P</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1553,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1622,7 +1628,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>26</v>
@@ -1640,7 +1646,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>26</v>

</xml_diff>